<commit_message>
result section and figures updated in ms
</commit_message>
<xml_diff>
--- a/results/Supplementary/6. PCA traits contributions to axis.xlsx
+++ b/results/Supplementary/6. PCA traits contributions to axis.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - Universidad de Oviedo\IMIB\Softwares\GitHub\movealong\results\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{BC7B50FE-0080-4D5A-8061-44AC0B863AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD1706F7-B229-4DC0-B654-44AD633B7213}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA7EA0E-15B6-4220-BC12-33E91CCB0BA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja4" sheetId="1" r:id="rId1"/>
+    <sheet name="2 subsets" sheetId="2" r:id="rId1"/>
+    <sheet name="4 subsets" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="38">
   <si>
     <t>TEMPERATE</t>
   </si>
@@ -111,13 +111,52 @@
   </si>
   <si>
     <t>Eigen values PCA without seed mass</t>
+  </si>
+  <si>
+    <t>BOTH SYSTEMS</t>
+  </si>
+  <si>
+    <t>$contrib</t>
+  </si>
+  <si>
+    <t>eigenvalue</t>
+  </si>
+  <si>
+    <t>comp 1</t>
+  </si>
+  <si>
+    <t>comp 2</t>
+  </si>
+  <si>
+    <t>comp 3</t>
+  </si>
+  <si>
+    <t>comp 4</t>
+  </si>
+  <si>
+    <t>comp 5</t>
+  </si>
+  <si>
+    <t>percentage of variance</t>
+  </si>
+  <si>
+    <t>cumulative percentage of variance</t>
+  </si>
+  <si>
+    <t>Dim.4</t>
+  </si>
+  <si>
+    <t>Dim.5</t>
+  </si>
+  <si>
+    <t>comp 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +169,32 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Lucida Sans Typewriter"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -168,8 +220,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFB9205"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002240"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -381,11 +457,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -400,61 +515,122 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,6 +639,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -480,6 +665,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFB9205"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -787,11 +977,960 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC297151-15B8-4CAA-B73A-C6957B1EEA3A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H25" sqref="G25:H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="60"/>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9">
+        <v>43.043571999999998</v>
+      </c>
+      <c r="D4" s="43">
+        <v>1.0400050000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2.4745916999999999</v>
+      </c>
+      <c r="F4" s="63"/>
+      <c r="G4" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="43">
+        <v>29.09958</v>
+      </c>
+      <c r="I4" s="43">
+        <v>26.778153</v>
+      </c>
+      <c r="J4" s="45">
+        <v>0.2351366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="60"/>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9">
+        <v>28.813271</v>
+      </c>
+      <c r="D5" s="10">
+        <v>20.719518999999998</v>
+      </c>
+      <c r="E5" s="45">
+        <v>2.9731597999999999</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="43">
+        <v>2.5558380000000001</v>
+      </c>
+      <c r="I5" s="43">
+        <v>3.4621225</v>
+      </c>
+      <c r="J5" s="46">
+        <v>81.763378599999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="43">
+        <v>3.570522</v>
+      </c>
+      <c r="D6" s="14">
+        <v>50.28593</v>
+      </c>
+      <c r="E6" s="11">
+        <v>3.9291527999999998</v>
+      </c>
+      <c r="F6" s="63"/>
+      <c r="G6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="9">
+        <v>32.139164999999998</v>
+      </c>
+      <c r="I6" s="43">
+        <v>9.1164821000000007</v>
+      </c>
+      <c r="J6" s="45">
+        <v>3.1236875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="60"/>
+      <c r="B7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="43">
+        <v>4.1743079999999999</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4.304996</v>
+      </c>
+      <c r="E7" s="47">
+        <v>90.004422899999994</v>
+      </c>
+      <c r="F7" s="63"/>
+      <c r="G7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="43">
+        <v>1.117211</v>
+      </c>
+      <c r="I7" s="14">
+        <v>59.748828699999997</v>
+      </c>
+      <c r="J7" s="45">
+        <v>11.640258899999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="61"/>
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="44">
+        <v>20.398326999999998</v>
+      </c>
+      <c r="D8" s="18">
+        <v>23.649549</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0.61867280000000002</v>
+      </c>
+      <c r="F8" s="64"/>
+      <c r="G8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="22">
+        <v>35.088206</v>
+      </c>
+      <c r="I8" s="44">
+        <v>0.89441369999999998</v>
+      </c>
+      <c r="J8" s="48">
+        <v>3.2375384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="41">
+        <v>2.11101472</v>
+      </c>
+      <c r="C11" s="41">
+        <v>42.220294000000003</v>
+      </c>
+      <c r="D11" s="41">
+        <v>42.220289999999999</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="37">
+        <v>1.9659093999999999</v>
+      </c>
+      <c r="H11" s="41">
+        <v>39.318187000000002</v>
+      </c>
+      <c r="I11" s="41">
+        <v>39.318190000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="41">
+        <v>1.35555282</v>
+      </c>
+      <c r="C12" s="41">
+        <v>27.111056000000001</v>
+      </c>
+      <c r="D12" s="41">
+        <v>69.33135</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="37">
+        <v>1.3702772000000001</v>
+      </c>
+      <c r="H12" s="41">
+        <v>27.405543999999999</v>
+      </c>
+      <c r="I12" s="41">
+        <v>66.723730000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="41">
+        <v>0.93995066999999999</v>
+      </c>
+      <c r="C13" s="41">
+        <v>18.799012999999999</v>
+      </c>
+      <c r="D13" s="41">
+        <v>88.130359999999996</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="37">
+        <v>1.0863970999999999</v>
+      </c>
+      <c r="H13" s="41">
+        <v>21.727943</v>
+      </c>
+      <c r="I13" s="41">
+        <v>88.451669999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="41">
+        <v>0.49700702000000002</v>
+      </c>
+      <c r="C14" s="41">
+        <v>9.9401399999999995</v>
+      </c>
+      <c r="D14" s="41">
+        <v>98.070499999999996</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="37">
+        <v>0.4626557</v>
+      </c>
+      <c r="H14" s="41">
+        <v>9.2531149999999993</v>
+      </c>
+      <c r="I14" s="41">
+        <v>97.704790000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="41">
+        <v>9.6474770000000001E-2</v>
+      </c>
+      <c r="C15" s="41">
+        <v>1.929495</v>
+      </c>
+      <c r="D15" s="41">
+        <v>100</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="37">
+        <v>0.1147606</v>
+      </c>
+      <c r="H15" s="41">
+        <v>2.2952110000000001</v>
+      </c>
+      <c r="I15" s="41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="60"/>
+      <c r="B21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="9">
+        <v>41.785922999999997</v>
+      </c>
+      <c r="D21" s="43">
+        <v>2.1427640000000001</v>
+      </c>
+      <c r="E21" s="45">
+        <v>1.8225370000000001</v>
+      </c>
+      <c r="F21" s="63"/>
+      <c r="G21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="43">
+        <v>8.8842130000000008</v>
+      </c>
+      <c r="I21" s="14">
+        <v>34.109564200000001</v>
+      </c>
+      <c r="J21" s="45">
+        <v>10.554693</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="60"/>
+      <c r="B22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="9">
+        <v>25.482738999999999</v>
+      </c>
+      <c r="D22" s="43">
+        <v>25.731169999999999</v>
+      </c>
+      <c r="E22" s="45">
+        <v>1.8952990000000001</v>
+      </c>
+      <c r="F22" s="63"/>
+      <c r="G22" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="43">
+        <v>4.8531959999999996</v>
+      </c>
+      <c r="I22" s="43">
+        <v>0.32394529999999999</v>
+      </c>
+      <c r="J22" s="47">
+        <v>66.537403999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="60"/>
+      <c r="B23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="43">
+        <v>4.2013199999999999</v>
+      </c>
+      <c r="D23" s="14">
+        <v>42.797263999999998</v>
+      </c>
+      <c r="E23" s="45">
+        <v>1.7051099999999999</v>
+      </c>
+      <c r="F23" s="63"/>
+      <c r="G23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="9">
+        <v>26.016293999999998</v>
+      </c>
+      <c r="I23" s="43">
+        <v>4.6919646000000004</v>
+      </c>
+      <c r="J23" s="45">
+        <v>12.509724</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="60"/>
+      <c r="B24" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="43">
+        <v>4.946123</v>
+      </c>
+      <c r="D24" s="43">
+        <v>2.204008</v>
+      </c>
+      <c r="E24" s="47">
+        <v>44.925671000000001</v>
+      </c>
+      <c r="F24" s="63"/>
+      <c r="G24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="43">
+        <v>18.476635000000002</v>
+      </c>
+      <c r="I24" s="14">
+        <v>28.466472599999999</v>
+      </c>
+      <c r="J24" s="45">
+        <v>2.6284719999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+      <c r="B25" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="50">
+        <v>20.431076999999998</v>
+      </c>
+      <c r="D25" s="50">
+        <v>20.044910000000002</v>
+      </c>
+      <c r="E25" s="51">
+        <v>3.6204800000000001</v>
+      </c>
+      <c r="F25" s="63"/>
+      <c r="G25" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="58">
+        <v>24.318861999999999</v>
+      </c>
+      <c r="I25" s="50">
+        <v>9.9276619999999998</v>
+      </c>
+      <c r="J25" s="51">
+        <v>4.386298</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="61"/>
+      <c r="B26" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="44">
+        <v>3.1528179999999999</v>
+      </c>
+      <c r="D26" s="44">
+        <v>7.0798829999999997</v>
+      </c>
+      <c r="E26" s="54">
+        <v>46.030901999999998</v>
+      </c>
+      <c r="F26" s="64"/>
+      <c r="G26" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="44">
+        <v>17.450800000000001</v>
+      </c>
+      <c r="I26" s="44">
+        <v>22.4803912</v>
+      </c>
+      <c r="J26" s="48">
+        <v>3.38341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="41"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>2.1272998400000001</v>
+      </c>
+      <c r="C29">
+        <v>35.454996999999999</v>
+      </c>
+      <c r="D29">
+        <v>35.454999999999998</v>
+      </c>
+      <c r="E29" s="41"/>
+      <c r="F29" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29">
+        <v>2.0703161099999998</v>
+      </c>
+      <c r="H29">
+        <v>34.505268999999998</v>
+      </c>
+      <c r="I29">
+        <v>34.505270000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>1.3974187300000001</v>
+      </c>
+      <c r="C30">
+        <v>23.290312</v>
+      </c>
+      <c r="D30">
+        <v>58.745310000000003</v>
+      </c>
+      <c r="E30" s="41"/>
+      <c r="F30" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30">
+        <v>1.78480846</v>
+      </c>
+      <c r="H30">
+        <v>29.746808000000001</v>
+      </c>
+      <c r="I30">
+        <v>64.252080000000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1.02976449</v>
+      </c>
+      <c r="C31">
+        <v>17.162742000000001</v>
+      </c>
+      <c r="D31">
+        <v>75.908050000000003</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31">
+        <v>1.20548681</v>
+      </c>
+      <c r="H31">
+        <v>20.091446999999999</v>
+      </c>
+      <c r="I31">
+        <v>84.343519999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0.85591965000000003</v>
+      </c>
+      <c r="C32">
+        <v>14.265326999999999</v>
+      </c>
+      <c r="D32">
+        <v>90.173379999999995</v>
+      </c>
+      <c r="E32" s="41"/>
+      <c r="F32" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32">
+        <v>0.51298385000000002</v>
+      </c>
+      <c r="H32">
+        <v>8.5497309999999995</v>
+      </c>
+      <c r="I32">
+        <v>92.893249999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0.49600371999999998</v>
+      </c>
+      <c r="C33">
+        <v>8.2667289999999998</v>
+      </c>
+      <c r="D33">
+        <v>98.440110000000004</v>
+      </c>
+      <c r="E33" s="41"/>
+      <c r="F33" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>0.33854669999999998</v>
+      </c>
+      <c r="H33">
+        <v>5.6424450000000004</v>
+      </c>
+      <c r="I33">
+        <v>98.535700000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>9.3593560000000006E-2</v>
+      </c>
+      <c r="C34">
+        <v>1.559893</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34" s="41"/>
+      <c r="F34" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34">
+        <v>8.7858060000000002E-2</v>
+      </c>
+      <c r="H34">
+        <v>1.4643010000000001</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="37"/>
+      <c r="G36" s="38"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="37"/>
+      <c r="F37" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="F39" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="37">
+        <v>8.8842130000000008</v>
+      </c>
+      <c r="H39">
+        <v>34.109564200000001</v>
+      </c>
+      <c r="I39">
+        <v>10.554693</v>
+      </c>
+      <c r="J39">
+        <v>1.662313E-2</v>
+      </c>
+      <c r="K39">
+        <v>15.621288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="37"/>
+      <c r="F40" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="37">
+        <v>4.8531959999999996</v>
+      </c>
+      <c r="H40">
+        <v>0.32394529999999999</v>
+      </c>
+      <c r="I40">
+        <v>66.537403999999995</v>
+      </c>
+      <c r="J40">
+        <v>5.8899139500000004</v>
+      </c>
+      <c r="K40">
+        <v>16.654714999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="37"/>
+      <c r="F41" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="37">
+        <v>26.016293999999998</v>
+      </c>
+      <c r="H41">
+        <v>4.6919646000000004</v>
+      </c>
+      <c r="I41">
+        <v>12.509724</v>
+      </c>
+      <c r="J41">
+        <v>40.481718919999999</v>
+      </c>
+      <c r="K41">
+        <v>1.93428</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="37"/>
+      <c r="F42" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="37">
+        <v>18.476635000000002</v>
+      </c>
+      <c r="H42">
+        <v>28.466472599999999</v>
+      </c>
+      <c r="I42">
+        <v>2.6284719999999999</v>
+      </c>
+      <c r="J42">
+        <v>3.2986380799999999</v>
+      </c>
+      <c r="K42">
+        <v>7.7341230000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="40"/>
+      <c r="F43" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="40">
+        <v>24.318861999999999</v>
+      </c>
+      <c r="H43">
+        <v>9.9276619999999998</v>
+      </c>
+      <c r="I43">
+        <v>4.386298</v>
+      </c>
+      <c r="J43">
+        <v>37.100492850000002</v>
+      </c>
+      <c r="K43">
+        <v>21.866527999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F44" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="38">
+        <v>17.450800000000001</v>
+      </c>
+      <c r="H44">
+        <v>22.4803912</v>
+      </c>
+      <c r="I44">
+        <v>3.38341</v>
+      </c>
+      <c r="J44">
+        <v>13.212613060000001</v>
+      </c>
+      <c r="K44">
+        <v>36.189067000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="F20:F26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,24 +1949,24 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="G2" s="39" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="75"/>
+      <c r="G2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="75"/>
       <c r="L2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="67" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
@@ -868,7 +2007,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="68"/>
       <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
@@ -910,7 +2049,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
@@ -952,7 +2091,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="68"/>
       <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
@@ -994,7 +2133,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
@@ -1036,7 +2175,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
@@ -1064,7 +2203,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="5"/>
@@ -1090,7 +2229,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="71"/>
       <c r="B10" s="13" t="s">
         <v>6</v>
       </c>
@@ -1117,7 +2256,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="15" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +2283,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="8" t="s">
         <v>8</v>
       </c>
@@ -1171,7 +2310,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
@@ -1198,7 +2337,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="21" t="s">
         <v>10</v>
       </c>
@@ -1231,18 +2370,18 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
-      <c r="G17" s="39" t="s">
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
+      <c r="G17" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="75"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="23"/>
@@ -1267,7 +2406,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="67" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -1297,7 +2436,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="68"/>
       <c r="B20" s="12" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +2463,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="13" t="s">
         <v>8</v>
       </c>
@@ -1351,7 +2490,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="15" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +2517,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="12" t="s">
         <v>10</v>
       </c>
@@ -1405,7 +2544,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="69"/>
       <c r="B24" s="17" t="s">
         <v>12</v>
       </c>
@@ -1433,7 +2572,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="70" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="29" t="s">
@@ -1463,7 +2602,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="13" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +2629,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
+      <c r="A27" s="71"/>
       <c r="B27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1517,7 +2656,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
+      <c r="A28" s="71"/>
       <c r="B28" s="8" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +2683,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="12" t="s">
         <v>10</v>
       </c>
@@ -1571,7 +2710,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
+      <c r="A30" s="72"/>
       <c r="B30" s="31" t="s">
         <v>12</v>
       </c>

</xml_diff>